<commit_message>
feat: added database, collection; added questions successfully
</commit_message>
<xml_diff>
--- a/test/Game 4 Good - Questions Input.xlsx
+++ b/test/Game 4 Good - Questions Input.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>type</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>a controversial statement that a debater supports or refutes with evidence and reasoning</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Reasoning</t>
@@ -234,7 +231,9 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -252,7 +251,9 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -270,7 +271,9 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -288,25 +291,29 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="H5" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
@@ -316,15 +323,17 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="H7" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
@@ -334,15 +343,17 @@
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -352,15 +363,17 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -370,15 +383,17 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="H10" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -388,15 +403,17 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="H11" s="1">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>